<commit_message>
added logic to pull new markets
</commit_message>
<xml_diff>
--- a/data/0x3c16b9efe5e4fc0ec3963f17c64a3dcbf7269207.xlsx
+++ b/data/0x3c16b9efe5e4fc0ec3963f17c64a3dcbf7269207.xlsx
@@ -445,33 +445,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2022-05-30 T 15:36:44 UTC</t>
+          <t>2022-05-30 T 18:36:33 UTC</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1899.48837437375</v>
+        <v>1905.94020055625</v>
       </c>
       <c r="C2" t="n">
-        <v>0.783385</v>
+        <v>0.7886609999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>1.272197</v>
+        <v>1.259291</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-05-30 T 15:36:44 UTC</t>
+          <t>2022-05-30 T 18:36:33 UTC</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1899.48837437375</v>
+        <v>1905.94020055625</v>
       </c>
       <c r="C3" t="n">
-        <v>0.783385</v>
+        <v>0.7886609999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>1.272197</v>
+        <v>1.259291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
playing with schedule times
</commit_message>
<xml_diff>
--- a/data/0x3c16b9efe5e4fc0ec3963f17c64a3dcbf7269207.xlsx
+++ b/data/0x3c16b9efe5e4fc0ec3963f17c64a3dcbf7269207.xlsx
@@ -445,33 +445,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2022-05-30 T 18:36:33 UTC</t>
+          <t>2022-05-30 T 21:36:43 UTC</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1905.94020055625</v>
+        <v>1919.638797075</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7886609999999999</v>
+        <v>0.800712</v>
       </c>
       <c r="D2" t="n">
-        <v>1.259291</v>
+        <v>1.232407</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-05-30 T 18:36:33 UTC</t>
+          <t>2022-05-30 T 21:36:43 UTC</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1905.94020055625</v>
+        <v>1919.638797075</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7886609999999999</v>
+        <v>0.800712</v>
       </c>
       <c r="D3" t="n">
-        <v>1.259291</v>
+        <v>1.232407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>